<commit_message>
move example values to the correct columns
</commit_message>
<xml_diff>
--- a/templates/dataplant/Genomics_assay.xlsx
+++ b/templates/dataplant/Genomics_assay.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="116">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>Illumina TrueSeq</t>
+  </si>
+  <si>
+    <t>v2</t>
   </si>
   <si>
     <t>ACTTGA</t>
@@ -1217,7 +1220,7 @@
         <v>91</v>
       </c>
       <c r="T2" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="U2" t="s">
         <v>91</v>
@@ -1226,7 +1229,7 @@
         <v>91</v>
       </c>
       <c r="W2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="X2" t="s">
         <v>91</v>
@@ -1244,7 +1247,7 @@
         <v>91</v>
       </c>
       <c r="AC2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="AD2" t="s">
         <v>91</v>
@@ -1280,7 +1283,7 @@
         <v>91</v>
       </c>
       <c r="AO2" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="AP2" t="s">
         <v>91</v>
@@ -1315,7 +1318,7 @@
         <v>91</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F3" t="s">
         <v>91</v>
@@ -1324,7 +1327,7 @@
         <v>91</v>
       </c>
       <c r="H3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I3" t="s">
         <v>91</v>
@@ -1333,7 +1336,7 @@
         <v>91</v>
       </c>
       <c r="K3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L3" t="s">
         <v>91</v>
@@ -1342,7 +1345,7 @@
         <v>91</v>
       </c>
       <c r="N3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="O3" t="s">
         <v>91</v>
@@ -1369,7 +1372,7 @@
         <v>91</v>
       </c>
       <c r="W3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="X3" t="s">
         <v>91</v>
@@ -1414,7 +1417,7 @@
         <v>91</v>
       </c>
       <c r="AL3" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="AM3" t="s">
         <v>91</v>
@@ -1423,7 +1426,7 @@
         <v>91</v>
       </c>
       <c r="AO3" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="AP3" t="s">
         <v>91</v>
@@ -1458,7 +1461,7 @@
         <v>91</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F4" t="s">
         <v>91</v>
@@ -1467,7 +1470,7 @@
         <v>91</v>
       </c>
       <c r="H4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I4" t="s">
         <v>91</v>
@@ -1476,7 +1479,7 @@
         <v>91</v>
       </c>
       <c r="K4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L4" t="s">
         <v>91</v>
@@ -1512,7 +1515,7 @@
         <v>91</v>
       </c>
       <c r="W4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="X4" t="s">
         <v>91</v>
@@ -1557,7 +1560,7 @@
         <v>91</v>
       </c>
       <c r="AL4" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="AM4" t="s">
         <v>91</v>
@@ -1566,7 +1569,7 @@
         <v>91</v>
       </c>
       <c r="AO4" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="AP4" t="s">
         <v>91</v>
@@ -1610,7 +1613,7 @@
         <v>91</v>
       </c>
       <c r="H5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I5" t="s">
         <v>91</v>
@@ -1753,7 +1756,7 @@
         <v>91</v>
       </c>
       <c r="H6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I6" t="s">
         <v>91</v>

</xml_diff>